<commit_message>
reverse array program finished
</commit_message>
<xml_diff>
--- a/final_450.xlsx
+++ b/final_450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bankopedia\love-babbar-dsa-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E115769E-CAD3-453B-9F05-3CBCE33E1ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="465">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1516,7 +1516,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1540,6 +1540,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1559,9 +1562,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1599,7 +1602,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1705,7 +1708,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1847,7 +1850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1858,17 +1861,17 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1901,8 +1904,8 @@
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
+      <c r="C6" s="11">
+        <v>45443</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">

</xml_diff>

<commit_message>
finished min max array
</commit_message>
<xml_diff>
--- a/final_450.xlsx
+++ b/final_450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bankopedia\love-babbar-dsa-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E115769E-CAD3-453B-9F05-3CBCE33E1ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB13055-47F4-4EE3-9359-EF04ACEA1A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="465">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1861,7 +1861,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1915,8 +1915,8 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
+      <c r="C7" s="11">
+        <v>45443</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">

</xml_diff>